<commit_message>
Scale PCA + doco
</commit_message>
<xml_diff>
--- a/LinearMorphometrics/data/Models.xlsx
+++ b/LinearMorphometrics/data/Models.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mickp\Desktop\Methods paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jim\uni\Papers and talks\Micks mimicry methods\LinearMorphometrics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490634FA-173F-4BA5-8E7A-D5A83AE1E690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="93">
   <si>
     <t>Unique ID</t>
   </si>
@@ -186,36 +185,6 @@
     <t>BBS103</t>
   </si>
   <si>
-    <t>SCS101</t>
-  </si>
-  <si>
-    <t>ABS102</t>
-  </si>
-  <si>
-    <t>FTS101</t>
-  </si>
-  <si>
-    <t>BAS101</t>
-  </si>
-  <si>
-    <t>MBS101</t>
-  </si>
-  <si>
-    <t>BRS101</t>
-  </si>
-  <si>
-    <t>MFS101</t>
-  </si>
-  <si>
-    <t>DNS101</t>
-  </si>
-  <si>
-    <t>DNS102</t>
-  </si>
-  <si>
-    <t>DNS103</t>
-  </si>
-  <si>
     <t>Leg II Femur: width</t>
   </si>
   <si>
@@ -300,15 +269,6 @@
     <t>Additional  notes</t>
   </si>
   <si>
-    <t>Iridomyrmex?</t>
-  </si>
-  <si>
-    <t>FTS101b</t>
-  </si>
-  <si>
-    <t>Unusually wide head relative to body</t>
-  </si>
-  <si>
     <t>Bulbous gaster</t>
   </si>
   <si>
@@ -349,18 +309,12 @@
   </si>
   <si>
     <t>Unusual ant relative to other ants (body shape)</t>
-  </si>
-  <si>
-    <t>Myrmecia?</t>
-  </si>
-  <si>
-    <t>Myrmeciinae</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -834,46 +788,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AT37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" customWidth="1"/>
-    <col min="8" max="8" width="11.54296875" customWidth="1"/>
-    <col min="15" max="15" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.90625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" customWidth="1"/>
     <col min="20" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="10.7265625" customWidth="1"/>
-    <col min="22" max="22" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.54296875" customWidth="1"/>
-    <col min="28" max="28" width="10.81640625" customWidth="1"/>
-    <col min="30" max="30" width="11.08984375" customWidth="1"/>
-    <col min="31" max="31" width="10.453125" customWidth="1"/>
-    <col min="32" max="32" width="11.1796875" customWidth="1"/>
-    <col min="34" max="34" width="10.26953125" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5703125" customWidth="1"/>
+    <col min="28" max="28" width="10.85546875" customWidth="1"/>
+    <col min="30" max="30" width="11.140625" customWidth="1"/>
+    <col min="31" max="31" width="10.42578125" customWidth="1"/>
+    <col min="32" max="32" width="11.140625" customWidth="1"/>
+    <col min="34" max="34" width="10.28515625" customWidth="1"/>
     <col min="35" max="35" width="10" customWidth="1"/>
-    <col min="36" max="36" width="11.1796875" customWidth="1"/>
-    <col min="38" max="38" width="15.1796875" customWidth="1"/>
-    <col min="39" max="39" width="14.90625" customWidth="1"/>
-    <col min="40" max="40" width="16.6328125" customWidth="1"/>
-    <col min="42" max="42" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.7265625" customWidth="1"/>
-    <col min="46" max="46" width="34.6328125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.140625" customWidth="1"/>
+    <col min="38" max="38" width="15.140625" customWidth="1"/>
+    <col min="39" max="39" width="14.85546875" customWidth="1"/>
+    <col min="40" max="40" width="16.5703125" customWidth="1"/>
+    <col min="42" max="42" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.7109375" customWidth="1"/>
+    <col min="46" max="46" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:46" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -890,127 +844,127 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="R1" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="O1" s="14" t="s">
+      <c r="AD1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF1" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM1" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR1" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="P1" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="U1" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y1" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA1" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB1" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC1" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE1" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF1" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG1" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH1" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI1" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ1" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AK1" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL1" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="AM1" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="AN1" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP1" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="AQ1" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="AR1" s="15" t="s">
+      <c r="AT1" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="AT1" s="17" t="s">
-        <v>88</v>
-      </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1165,10 +1119,10 @@
         <v>0.61229620676474916</v>
       </c>
       <c r="AT2" s="20" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1278,7 +1232,7 @@
         <v>0.58099999999999996</v>
       </c>
       <c r="AG3" s="18">
-        <f t="shared" ref="AG3:AG48" si="19">J3</f>
+        <f t="shared" ref="AG3:AG37" si="19">J3</f>
         <v>1.956</v>
       </c>
       <c r="AH3" s="18">
@@ -1307,7 +1261,7 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="AO3" s="18">
-        <f t="shared" ref="AO3:AO48" si="20">Q3</f>
+        <f t="shared" ref="AO3:AO37" si="20">Q3</f>
         <v>2.3119999999999998</v>
       </c>
       <c r="AP3" s="18">
@@ -1323,7 +1277,7 @@
         <v>0.6255915828566424</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1478,7 +1432,7 @@
         <v>0.61443880673190199</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1633,7 +1587,7 @@
         <v>0.60575499958769619</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1788,7 +1742,7 @@
         <v>0.63086882710614423</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1943,10 +1897,10 @@
         <v>0.59604627527663923</v>
       </c>
       <c r="AT7" s="20" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -2101,10 +2055,10 @@
         <v>0.60871392230853605</v>
       </c>
       <c r="AT8" s="20" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -2259,10 +2213,10 @@
         <v>0.6189675879477482</v>
       </c>
       <c r="AT9" s="20" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
@@ -2417,7 +2371,7 @@
         <v>0.6577239219922274</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -2572,7 +2526,7 @@
         <v>0.58561988382802843</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
@@ -2727,7 +2681,7 @@
         <v>0.63331868120279178</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -2882,7 +2836,7 @@
         <v>0.5839654345726053</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -3037,7 +2991,7 @@
         <v>0.65082508250746063</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -3192,7 +3146,7 @@
         <v>0.63984696858129608</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -3347,7 +3301,7 @@
         <v>0.58401630741038857</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -3502,10 +3456,10 @@
         <v>0.60097296799148414</v>
       </c>
       <c r="AT17" s="4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -3660,7 +3614,7 @@
         <v>0.63383055678958322</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -3815,7 +3769,7 @@
         <v>0.63137187700720154</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
@@ -3970,10 +3924,10 @@
         <v>0.65004848839655061</v>
       </c>
       <c r="AT20" s="4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>34</v>
       </c>
@@ -4128,7 +4082,7 @@
         <v>0.65574985505114702</v>
       </c>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>35</v>
       </c>
@@ -4283,7 +4237,7 @@
         <v>0.64236357409706901</v>
       </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>36</v>
       </c>
@@ -4438,7 +4392,7 @@
         <v>0.61789750557648393</v>
       </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>37</v>
       </c>
@@ -4593,7 +4547,7 @@
         <v>0.60384289612057684</v>
       </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -4748,7 +4702,7 @@
         <v>0.63568745865956822</v>
       </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>39</v>
       </c>
@@ -4903,7 +4857,7 @@
         <v>0.62195137225920816</v>
       </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>40</v>
       </c>
@@ -5058,7 +5012,7 @@
         <v>0.61249809419138979</v>
       </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>41</v>
       </c>
@@ -5213,10 +5167,10 @@
         <v>0.61171490968307474</v>
       </c>
       <c r="AT28" s="20" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -5371,7 +5325,7 @@
         <v>0.59625086634705238</v>
       </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
@@ -5526,7 +5480,7 @@
         <v>0.62732547022095375</v>
       </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
@@ -5681,7 +5635,7 @@
         <v>0.61389865388820852</v>
       </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
@@ -5836,7 +5790,7 @@
         <v>0.60794174134868351</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
@@ -5988,7 +5942,7 @@
         <v>0.60909089226154223</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
@@ -6011,11 +5965,11 @@
         <v>1.952</v>
       </c>
       <c r="H34" s="18">
-        <f t="shared" ref="H34:H48" si="21">F34/G34</f>
+        <f t="shared" ref="H34:H37" si="21">F34/G34</f>
         <v>0.1403688524590164</v>
       </c>
       <c r="I34" s="18">
-        <f t="shared" ref="I34:I48" si="22">1-H34</f>
+        <f t="shared" ref="I34:I37" si="22">1-H34</f>
         <v>0.85963114754098358</v>
       </c>
       <c r="J34" s="18">
@@ -6031,15 +5985,15 @@
         <v>3.012</v>
       </c>
       <c r="N34" s="18">
-        <f t="shared" ref="N34:N48" si="23">L34+M34</f>
+        <f t="shared" ref="N34:N37" si="23">L34+M34</f>
         <v>4.7350000000000003</v>
       </c>
       <c r="O34" s="18">
-        <f t="shared" ref="O34:O48" si="24">J34/N34</f>
+        <f t="shared" ref="O34:O37" si="24">J34/N34</f>
         <v>0.37571277719112983</v>
       </c>
       <c r="P34" s="18">
-        <f t="shared" ref="P34:P48" si="25">1-O34</f>
+        <f t="shared" ref="P34:P37" si="25">1-O34</f>
         <v>0.62428722280887017</v>
       </c>
       <c r="Q34" s="18">
@@ -6055,15 +6009,15 @@
         <v>0.71799999999999997</v>
       </c>
       <c r="U34" s="18">
-        <f t="shared" ref="U34:U48" si="26">S34+T34</f>
+        <f t="shared" ref="U34:U37" si="26">S34+T34</f>
         <v>3.452</v>
       </c>
       <c r="V34" s="18">
-        <f t="shared" ref="V34:V48" si="27">Q34/U34</f>
+        <f t="shared" ref="V34:V37" si="27">Q34/U34</f>
         <v>0.67728852838933951</v>
       </c>
       <c r="W34" s="18">
-        <f t="shared" ref="W34:W48" si="28">1-V34</f>
+        <f t="shared" ref="W34:W37" si="28">1-V34</f>
         <v>0.32271147161066049</v>
       </c>
       <c r="X34" s="18">
@@ -6073,11 +6027,11 @@
         <v>0.17100000000000001</v>
       </c>
       <c r="Z34" s="18">
-        <f t="shared" ref="Z34:Z48" si="29">L34+M34+S34+T34+Y34</f>
+        <f t="shared" ref="Z34:Z37" si="29">L34+M34+S34+T34+Y34</f>
         <v>8.3580000000000005</v>
       </c>
       <c r="AA34" s="18">
-        <f t="shared" ref="AA34:AA48" si="30">Y34/Z34</f>
+        <f t="shared" ref="AA34:AA37" si="30">Y34/Z34</f>
         <v>2.0459440057430008E-2</v>
       </c>
       <c r="AB34" s="18">
@@ -6087,11 +6041,11 @@
         <v>1.2130000000000001</v>
       </c>
       <c r="AD34" s="18">
-        <f t="shared" ref="AD34:AD48" si="31">AB34/AC34</f>
+        <f t="shared" ref="AD34:AD37" si="31">AB34/AC34</f>
         <v>0.35284418796372624</v>
       </c>
       <c r="AE34" s="18">
-        <f t="shared" ref="AE34:AE48" si="32">1-AD34</f>
+        <f t="shared" ref="AE34:AE37" si="32">1-AD34</f>
         <v>0.6471558120362737</v>
       </c>
       <c r="AF34" s="18">
@@ -6102,11 +6056,11 @@
         <v>1.7789999999999999</v>
       </c>
       <c r="AH34" s="18">
-        <f t="shared" ref="AH34:AH48" si="33">AF34/AG34</f>
+        <f t="shared" ref="AH34:AH37" si="33">AF34/AG34</f>
         <v>0.3215289488476672</v>
       </c>
       <c r="AI34" s="18">
-        <f t="shared" ref="AI34:AI48" si="34">1-AH34</f>
+        <f t="shared" ref="AI34:AI37" si="34">1-AH34</f>
         <v>0.67847105115233286</v>
       </c>
       <c r="AJ34" s="18">
@@ -6116,11 +6070,11 @@
         <v>1.8069999999999999</v>
       </c>
       <c r="AL34" s="18">
-        <f t="shared" ref="AL34:AL48" si="35">AJ34/AK34</f>
+        <f t="shared" ref="AL34:AL37" si="35">AJ34/AK34</f>
         <v>0.17930271167681242</v>
       </c>
       <c r="AM34" s="18">
-        <f t="shared" ref="AM34:AM48" si="36">1-AL34</f>
+        <f t="shared" ref="AM34:AM37" si="36">1-AL34</f>
         <v>0.82069728832318756</v>
       </c>
       <c r="AN34" s="18">
@@ -6131,19 +6085,19 @@
         <v>2.3380000000000001</v>
       </c>
       <c r="AP34" s="18">
-        <f t="shared" ref="AP34:AP48" si="37">AN34/AO34</f>
+        <f t="shared" ref="AP34:AP37" si="37">AN34/AO34</f>
         <v>0.14756201881950384</v>
       </c>
       <c r="AQ34" s="18">
-        <f t="shared" ref="AQ34:AQ48" si="38">1-AP34</f>
+        <f t="shared" ref="AQ34:AQ37" si="38">1-AP34</f>
         <v>0.85243798118049618</v>
       </c>
       <c r="AR34" s="18">
-        <f t="shared" ref="AR34:AR48" si="39">(I34+P34+W34+AA34+AE34+AI34+AM34+AQ34)/8</f>
+        <f t="shared" ref="AR34:AR37" si="39">(I34+P34+W34+AA34+AE34+AI34+AM34+AQ34)/8</f>
         <v>0.60323142683877928</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
@@ -6298,10 +6252,10 @@
         <v>0.55376995676210106</v>
       </c>
       <c r="AT35" s="20" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
@@ -6456,7 +6410,7 @@
         <v>0.6238556883634423</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
@@ -6611,1719 +6565,11 @@
         <v>0.59983414162493176</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" s="18">
-        <v>0.34300000000000003</v>
-      </c>
-      <c r="G38" s="18">
-        <v>2.9359999999999999</v>
-      </c>
-      <c r="H38" s="18">
-        <f t="shared" si="21"/>
-        <v>0.11682561307901909</v>
-      </c>
-      <c r="I38" s="18">
-        <f t="shared" si="22"/>
-        <v>0.88317438692098094</v>
-      </c>
-      <c r="J38" s="18">
-        <v>2.0760000000000001</v>
-      </c>
-      <c r="K38" s="18">
-        <v>1.51</v>
-      </c>
-      <c r="L38" s="18">
-        <v>2.5459999999999998</v>
-      </c>
-      <c r="M38" s="18">
-        <v>3.62</v>
-      </c>
-      <c r="N38" s="18">
-        <f t="shared" si="23"/>
-        <v>6.1660000000000004</v>
-      </c>
-      <c r="O38" s="18">
-        <f t="shared" si="24"/>
-        <v>0.33668504703211155</v>
-      </c>
-      <c r="P38" s="18">
-        <f t="shared" si="25"/>
-        <v>0.66331495296788845</v>
-      </c>
-      <c r="Q38" s="18">
-        <v>1.86</v>
-      </c>
-      <c r="R38" s="18">
-        <v>0.501</v>
-      </c>
-      <c r="S38" s="18">
-        <v>4.4240000000000004</v>
-      </c>
-      <c r="T38" s="18">
-        <v>0.66200000000000003</v>
-      </c>
-      <c r="U38" s="18">
-        <f t="shared" si="26"/>
-        <v>5.0860000000000003</v>
-      </c>
-      <c r="V38" s="18">
-        <f t="shared" si="27"/>
-        <v>0.36570979158474243</v>
-      </c>
-      <c r="W38" s="18">
-        <f t="shared" si="28"/>
-        <v>0.63429020841525752</v>
-      </c>
-      <c r="X38" s="18">
-        <v>0.28299999999999997</v>
-      </c>
-      <c r="Y38" s="18">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="Z38" s="18">
-        <f t="shared" si="29"/>
-        <v>11.487</v>
-      </c>
-      <c r="AA38" s="18">
-        <f t="shared" si="30"/>
-        <v>2.0457908940541482E-2</v>
-      </c>
-      <c r="AB38" s="18">
-        <v>0.58099999999999996</v>
-      </c>
-      <c r="AC38" s="18">
-        <v>1.544</v>
-      </c>
-      <c r="AD38" s="18">
-        <f t="shared" si="31"/>
-        <v>0.37629533678756472</v>
-      </c>
-      <c r="AE38" s="18">
-        <f t="shared" si="32"/>
-        <v>0.62370466321243523</v>
-      </c>
-      <c r="AF38" s="18">
-        <v>0.76300000000000001</v>
-      </c>
-      <c r="AG38" s="18">
-        <f t="shared" si="19"/>
-        <v>2.0760000000000001</v>
-      </c>
-      <c r="AH38" s="18">
-        <f t="shared" si="33"/>
-        <v>0.36753371868978807</v>
-      </c>
-      <c r="AI38" s="18">
-        <f t="shared" si="34"/>
-        <v>0.63246628131021199</v>
-      </c>
-      <c r="AJ38" s="18">
-        <v>0.373</v>
-      </c>
-      <c r="AK38" s="18">
-        <v>1.8660000000000001</v>
-      </c>
-      <c r="AL38" s="18">
-        <f t="shared" si="35"/>
-        <v>0.19989281886387994</v>
-      </c>
-      <c r="AM38" s="18">
-        <f t="shared" si="36"/>
-        <v>0.80010718113612</v>
-      </c>
-      <c r="AN38" s="18">
-        <v>0.45800000000000002</v>
-      </c>
-      <c r="AO38" s="18">
-        <f t="shared" si="20"/>
-        <v>1.86</v>
-      </c>
-      <c r="AP38" s="18">
-        <f t="shared" si="37"/>
-        <v>0.24623655913978496</v>
-      </c>
-      <c r="AQ38" s="18">
-        <f t="shared" si="38"/>
-        <v>0.75376344086021507</v>
-      </c>
-      <c r="AR38" s="18">
-        <f t="shared" si="39"/>
-        <v>0.62640987797045633</v>
-      </c>
-    </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F39" s="18">
-        <v>0.152</v>
-      </c>
-      <c r="G39" s="18">
-        <v>0.84299999999999997</v>
-      </c>
-      <c r="H39" s="18">
-        <f t="shared" si="21"/>
-        <v>0.18030842230130487</v>
-      </c>
-      <c r="I39" s="18">
-        <f t="shared" si="22"/>
-        <v>0.81969157769869516</v>
-      </c>
-      <c r="J39" s="18">
-        <v>1</v>
-      </c>
-      <c r="K39" s="18">
-        <v>0.58099999999999996</v>
-      </c>
-      <c r="L39" s="18">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="M39" s="18">
-        <v>1.1919999999999999</v>
-      </c>
-      <c r="N39" s="18">
-        <f t="shared" si="23"/>
-        <v>2.1150000000000002</v>
-      </c>
-      <c r="O39" s="18">
-        <f t="shared" si="24"/>
-        <v>0.47281323877068554</v>
-      </c>
-      <c r="P39" s="18">
-        <f t="shared" si="25"/>
-        <v>0.5271867612293144</v>
-      </c>
-      <c r="Q39" s="18">
-        <v>1.1060000000000001</v>
-      </c>
-      <c r="R39" s="18">
-        <v>0.32700000000000001</v>
-      </c>
-      <c r="S39" s="18">
-        <v>1.4419999999999999</v>
-      </c>
-      <c r="T39" s="18">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="U39" s="18">
-        <f t="shared" si="26"/>
-        <v>1.907</v>
-      </c>
-      <c r="V39" s="18">
-        <f t="shared" si="27"/>
-        <v>0.57996853696906137</v>
-      </c>
-      <c r="W39" s="18">
-        <f t="shared" si="28"/>
-        <v>0.42003146303093863</v>
-      </c>
-      <c r="X39" s="18">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="Y39" s="18">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="Z39" s="18">
-        <f t="shared" si="29"/>
-        <v>4.1180000000000003</v>
-      </c>
-      <c r="AA39" s="18">
-        <f t="shared" si="30"/>
-        <v>2.3312287518212724E-2</v>
-      </c>
-      <c r="AB39" s="18">
-        <v>0.23799999999999999</v>
-      </c>
-      <c r="AC39" s="18">
-        <v>0.61499999999999999</v>
-      </c>
-      <c r="AD39" s="18">
-        <f t="shared" si="31"/>
-        <v>0.38699186991869916</v>
-      </c>
-      <c r="AE39" s="18">
-        <f t="shared" si="32"/>
-        <v>0.61300813008130084</v>
-      </c>
-      <c r="AF39" s="18">
-        <v>0.307</v>
-      </c>
-      <c r="AG39" s="18">
-        <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-      <c r="AH39" s="18">
-        <f t="shared" si="33"/>
-        <v>0.307</v>
-      </c>
-      <c r="AI39" s="18">
-        <f t="shared" si="34"/>
-        <v>0.69300000000000006</v>
-      </c>
-      <c r="AJ39" s="18">
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="AK39" s="18">
-        <v>0.83799999999999997</v>
-      </c>
-      <c r="AL39" s="18">
-        <f t="shared" si="35"/>
-        <v>0.15990453460620527</v>
-      </c>
-      <c r="AM39" s="18">
-        <f t="shared" si="36"/>
-        <v>0.84009546539379476</v>
-      </c>
-      <c r="AN39" s="18">
-        <v>0.28299999999999997</v>
-      </c>
-      <c r="AO39" s="18">
-        <f t="shared" si="20"/>
-        <v>1.1060000000000001</v>
-      </c>
-      <c r="AP39" s="18">
-        <f t="shared" si="37"/>
-        <v>0.25587703435804698</v>
-      </c>
-      <c r="AQ39" s="18">
-        <f t="shared" si="38"/>
-        <v>0.74412296564195302</v>
-      </c>
-      <c r="AR39" s="18">
-        <f t="shared" si="39"/>
-        <v>0.58505608132427622</v>
-      </c>
-    </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" s="18">
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="G40" s="18">
-        <v>3.915</v>
-      </c>
-      <c r="H40" s="18">
-        <f t="shared" si="21"/>
-        <v>0.10140485312899107</v>
-      </c>
-      <c r="I40" s="18">
-        <f t="shared" si="22"/>
-        <v>0.89859514687100894</v>
-      </c>
-      <c r="J40" s="18">
-        <v>1.2470000000000001</v>
-      </c>
-      <c r="K40" s="18">
-        <v>1.05</v>
-      </c>
-      <c r="L40" s="18">
-        <v>2.028</v>
-      </c>
-      <c r="M40" s="18">
-        <v>3.915</v>
-      </c>
-      <c r="N40" s="18">
-        <f t="shared" si="23"/>
-        <v>5.9429999999999996</v>
-      </c>
-      <c r="O40" s="18">
-        <f t="shared" si="24"/>
-        <v>0.20982668685848901</v>
-      </c>
-      <c r="P40" s="18">
-        <f t="shared" si="25"/>
-        <v>0.79017331314151096</v>
-      </c>
-      <c r="Q40" s="18">
-        <v>1.43</v>
-      </c>
-      <c r="R40" s="18">
-        <v>0.376</v>
-      </c>
-      <c r="S40" s="18">
-        <v>2.4359999999999999</v>
-      </c>
-      <c r="T40" s="18">
-        <v>0.59699999999999998</v>
-      </c>
-      <c r="U40" s="18">
-        <f t="shared" si="26"/>
-        <v>3.0329999999999999</v>
-      </c>
-      <c r="V40" s="18">
-        <f t="shared" si="27"/>
-        <v>0.47148038245961094</v>
-      </c>
-      <c r="W40" s="18">
-        <f t="shared" si="28"/>
-        <v>0.52851961754038901</v>
-      </c>
-      <c r="X40" s="18">
-        <v>0.24</v>
-      </c>
-      <c r="Y40" s="18">
-        <v>0.153</v>
-      </c>
-      <c r="Z40" s="18">
-        <f t="shared" si="29"/>
-        <v>9.1289999999999996</v>
-      </c>
-      <c r="AA40" s="18">
-        <f t="shared" si="30"/>
-        <v>1.6759776536312849E-2</v>
-      </c>
-      <c r="AB40" s="18">
-        <v>0.44900000000000001</v>
-      </c>
-      <c r="AC40" s="18">
-        <v>1.022</v>
-      </c>
-      <c r="AD40" s="18">
-        <f t="shared" si="31"/>
-        <v>0.43933463796477495</v>
-      </c>
-      <c r="AE40" s="18">
-        <f t="shared" si="32"/>
-        <v>0.5606653620352251</v>
-      </c>
-      <c r="AF40" s="18">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="AG40" s="18">
-        <f t="shared" si="19"/>
-        <v>1.2470000000000001</v>
-      </c>
-      <c r="AH40" s="18">
-        <f t="shared" si="33"/>
-        <v>0.34001603849238166</v>
-      </c>
-      <c r="AI40" s="18">
-        <f t="shared" si="34"/>
-        <v>0.6599839615076184</v>
-      </c>
-      <c r="AJ40" s="18">
-        <v>0.314</v>
-      </c>
-      <c r="AK40" s="18">
-        <v>1.377</v>
-      </c>
-      <c r="AL40" s="18">
-        <f t="shared" si="35"/>
-        <v>0.22803195352214961</v>
-      </c>
-      <c r="AM40" s="18">
-        <f t="shared" si="36"/>
-        <v>0.77196804647785044</v>
-      </c>
-      <c r="AN40" s="18">
-        <v>0.373</v>
-      </c>
-      <c r="AO40" s="18">
-        <f t="shared" si="20"/>
-        <v>1.43</v>
-      </c>
-      <c r="AP40" s="18">
-        <f t="shared" si="37"/>
-        <v>0.26083916083916087</v>
-      </c>
-      <c r="AQ40" s="18">
-        <f t="shared" si="38"/>
-        <v>0.73916083916083908</v>
-      </c>
-      <c r="AR40" s="18">
-        <f t="shared" si="39"/>
-        <v>0.62072825790884445</v>
-      </c>
-    </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F41" s="18">
-        <v>0.188</v>
-      </c>
-      <c r="G41" s="18">
-        <v>1.35</v>
-      </c>
-      <c r="H41" s="18">
-        <f t="shared" si="21"/>
-        <v>0.13925925925925925</v>
-      </c>
-      <c r="I41" s="18">
-        <f t="shared" si="22"/>
-        <v>0.86074074074074081</v>
-      </c>
-      <c r="J41" s="18">
-        <v>1.169</v>
-      </c>
-      <c r="K41" s="18">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="L41" s="18">
-        <v>1.4219999999999999</v>
-      </c>
-      <c r="M41" s="18">
-        <v>1.8680000000000001</v>
-      </c>
-      <c r="N41" s="18">
-        <f t="shared" si="23"/>
-        <v>3.29</v>
-      </c>
-      <c r="O41" s="18">
-        <f t="shared" si="24"/>
-        <v>0.35531914893617023</v>
-      </c>
-      <c r="P41" s="18">
-        <f t="shared" si="25"/>
-        <v>0.64468085106382977</v>
-      </c>
-      <c r="Q41" s="18">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="R41" s="18">
-        <v>0.495</v>
-      </c>
-      <c r="S41" s="18">
-        <v>1.7370000000000001</v>
-      </c>
-      <c r="T41" s="18">
-        <v>0.52200000000000002</v>
-      </c>
-      <c r="U41" s="18">
-        <f t="shared" si="26"/>
-        <v>2.2590000000000003</v>
-      </c>
-      <c r="V41" s="18">
-        <f t="shared" si="27"/>
-        <v>0.42009738822487819</v>
-      </c>
-      <c r="W41" s="18">
-        <f t="shared" si="28"/>
-        <v>0.57990261177512181</v>
-      </c>
-      <c r="X41" s="18">
-        <v>0.23799999999999999</v>
-      </c>
-      <c r="Y41" s="18">
-        <v>0.247</v>
-      </c>
-      <c r="Z41" s="18">
-        <f t="shared" si="29"/>
-        <v>5.7960000000000003</v>
-      </c>
-      <c r="AA41" s="18">
-        <f t="shared" si="30"/>
-        <v>4.2615596963423048E-2</v>
-      </c>
-      <c r="AB41" s="18">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="AC41" s="18">
-        <v>0.86099999999999999</v>
-      </c>
-      <c r="AD41" s="18">
-        <f t="shared" si="31"/>
-        <v>0.49361207897793263</v>
-      </c>
-      <c r="AE41" s="18">
-        <f t="shared" si="32"/>
-        <v>0.50638792102206742</v>
-      </c>
-      <c r="AF41" s="18">
-        <v>0.504</v>
-      </c>
-      <c r="AG41" s="18">
-        <f t="shared" si="19"/>
-        <v>1.169</v>
-      </c>
-      <c r="AH41" s="18">
-        <f t="shared" si="33"/>
-        <v>0.43113772455089822</v>
-      </c>
-      <c r="AI41" s="18">
-        <f t="shared" si="34"/>
-        <v>0.56886227544910173</v>
-      </c>
-      <c r="AJ41" s="18">
-        <v>0.35899999999999999</v>
-      </c>
-      <c r="AK41" s="18">
-        <v>0.94</v>
-      </c>
-      <c r="AL41" s="18">
-        <f t="shared" si="35"/>
-        <v>0.3819148936170213</v>
-      </c>
-      <c r="AM41" s="18">
-        <f t="shared" si="36"/>
-        <v>0.61808510638297864</v>
-      </c>
-      <c r="AN41" s="18">
-        <v>0.39200000000000002</v>
-      </c>
-      <c r="AO41" s="18">
-        <f t="shared" si="20"/>
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="AP41" s="18">
-        <f t="shared" si="37"/>
-        <v>0.41306638566912546</v>
-      </c>
-      <c r="AQ41" s="18">
-        <f t="shared" si="38"/>
-        <v>0.58693361433087454</v>
-      </c>
-      <c r="AR41" s="18">
-        <f t="shared" si="39"/>
-        <v>0.5510260897160173</v>
-      </c>
-    </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="18">
-        <v>0.36</v>
-      </c>
-      <c r="G42" s="18">
-        <v>2.71</v>
-      </c>
-      <c r="H42" s="18">
-        <f t="shared" si="21"/>
-        <v>0.13284132841328414</v>
-      </c>
-      <c r="I42" s="18">
-        <f t="shared" si="22"/>
-        <v>0.86715867158671589</v>
-      </c>
-      <c r="J42" s="18">
-        <v>2.8</v>
-      </c>
-      <c r="K42" s="18">
-        <v>1.619</v>
-      </c>
-      <c r="L42" s="18">
-        <v>2.8239999999999998</v>
-      </c>
-      <c r="M42" s="18">
-        <v>5.5010000000000003</v>
-      </c>
-      <c r="N42" s="18">
-        <f t="shared" si="23"/>
-        <v>8.3249999999999993</v>
-      </c>
-      <c r="O42" s="18">
-        <f t="shared" si="24"/>
-        <v>0.33633633633633636</v>
-      </c>
-      <c r="P42" s="18">
-        <f t="shared" si="25"/>
-        <v>0.66366366366366369</v>
-      </c>
-      <c r="Q42" s="18">
-        <v>2.742</v>
-      </c>
-      <c r="R42" s="18">
-        <v>1.3720000000000001</v>
-      </c>
-      <c r="S42" s="18">
-        <v>3.7789999999999999</v>
-      </c>
-      <c r="T42" s="18">
-        <v>1.4019999999999999</v>
-      </c>
-      <c r="U42" s="18">
-        <f t="shared" si="26"/>
-        <v>5.181</v>
-      </c>
-      <c r="V42" s="18">
-        <f t="shared" si="27"/>
-        <v>0.52924145917776488</v>
-      </c>
-      <c r="W42" s="18">
-        <f t="shared" si="28"/>
-        <v>0.47075854082223512</v>
-      </c>
-      <c r="X42" s="18">
-        <v>0.442</v>
-      </c>
-      <c r="Y42" s="18">
-        <v>1.5229999999999999</v>
-      </c>
-      <c r="Z42" s="18">
-        <f t="shared" si="29"/>
-        <v>15.028999999999998</v>
-      </c>
-      <c r="AA42" s="18">
-        <f t="shared" si="30"/>
-        <v>0.10133741433229092</v>
-      </c>
-      <c r="AB42" s="18">
-        <v>0.73099999999999998</v>
-      </c>
-      <c r="AC42" s="18">
-        <v>2.0670000000000002</v>
-      </c>
-      <c r="AD42" s="18">
-        <f t="shared" si="31"/>
-        <v>0.35365263667150454</v>
-      </c>
-      <c r="AE42" s="18">
-        <f t="shared" si="32"/>
-        <v>0.64634736332849552</v>
-      </c>
-      <c r="AF42" s="18">
-        <v>0.69299999999999995</v>
-      </c>
-      <c r="AG42" s="18">
-        <f t="shared" si="19"/>
-        <v>2.8</v>
-      </c>
-      <c r="AH42" s="18">
-        <f t="shared" si="33"/>
-        <v>0.2475</v>
-      </c>
-      <c r="AI42" s="18">
-        <f t="shared" si="34"/>
-        <v>0.75249999999999995</v>
-      </c>
-      <c r="AJ42" s="18">
-        <v>1.2330000000000001</v>
-      </c>
-      <c r="AK42" s="18">
-        <v>2.5209999999999999</v>
-      </c>
-      <c r="AL42" s="18">
-        <f t="shared" si="35"/>
-        <v>0.4890916303054344</v>
-      </c>
-      <c r="AM42" s="18">
-        <f t="shared" si="36"/>
-        <v>0.51090836969456555</v>
-      </c>
-      <c r="AN42" s="18">
-        <v>1.3859999999999999</v>
-      </c>
-      <c r="AO42" s="18">
-        <f t="shared" si="20"/>
-        <v>2.742</v>
-      </c>
-      <c r="AP42" s="18">
-        <f t="shared" si="37"/>
-        <v>0.50547045951859948</v>
-      </c>
-      <c r="AQ42" s="18">
-        <f t="shared" si="38"/>
-        <v>0.49452954048140052</v>
-      </c>
-      <c r="AR42" s="18">
-        <f t="shared" si="39"/>
-        <v>0.56340044548867096</v>
-      </c>
-    </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F43" s="18">
-        <v>0.48299999999999998</v>
-      </c>
-      <c r="G43" s="18">
-        <v>3.9239999999999999</v>
-      </c>
-      <c r="H43" s="18">
-        <f t="shared" si="21"/>
-        <v>0.12308868501529052</v>
-      </c>
-      <c r="I43" s="18">
-        <f t="shared" si="22"/>
-        <v>0.87691131498470942</v>
-      </c>
-      <c r="J43" s="18">
-        <v>2.8039999999999998</v>
-      </c>
-      <c r="K43" s="18">
-        <v>1.9910000000000001</v>
-      </c>
-      <c r="L43" s="18">
-        <v>3.0539999999999998</v>
-      </c>
-      <c r="M43" s="18">
-        <v>5.5819999999999999</v>
-      </c>
-      <c r="N43" s="18">
-        <f t="shared" si="23"/>
-        <v>8.6359999999999992</v>
-      </c>
-      <c r="O43" s="18">
-        <f t="shared" si="24"/>
-        <v>0.32468735525706344</v>
-      </c>
-      <c r="P43" s="18">
-        <f t="shared" si="25"/>
-        <v>0.67531264474293651</v>
-      </c>
-      <c r="Q43" s="18">
-        <v>3.1360000000000001</v>
-      </c>
-      <c r="R43" s="18">
-        <v>0.79100000000000004</v>
-      </c>
-      <c r="S43" s="18">
-        <v>4.8570000000000002</v>
-      </c>
-      <c r="T43" s="18">
-        <v>1.2170000000000001</v>
-      </c>
-      <c r="U43" s="18">
-        <f t="shared" si="26"/>
-        <v>6.0739999999999998</v>
-      </c>
-      <c r="V43" s="18">
-        <f t="shared" si="27"/>
-        <v>0.51629897925584467</v>
-      </c>
-      <c r="W43" s="18">
-        <f t="shared" si="28"/>
-        <v>0.48370102074415533</v>
-      </c>
-      <c r="X43" s="18">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="Y43" s="18">
-        <v>0.193</v>
-      </c>
-      <c r="Z43" s="18">
-        <f t="shared" si="29"/>
-        <v>14.902999999999999</v>
-      </c>
-      <c r="AA43" s="18">
-        <f t="shared" si="30"/>
-        <v>1.2950412668590218E-2</v>
-      </c>
-      <c r="AB43" s="18">
-        <v>0.61</v>
-      </c>
-      <c r="AC43" s="18">
-        <v>2.052</v>
-      </c>
-      <c r="AD43" s="18">
-        <f t="shared" si="31"/>
-        <v>0.29727095516569202</v>
-      </c>
-      <c r="AE43" s="18">
-        <f t="shared" si="32"/>
-        <v>0.70272904483430798</v>
-      </c>
-      <c r="AF43" s="18">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="AG43" s="18">
-        <f t="shared" si="19"/>
-        <v>2.8039999999999998</v>
-      </c>
-      <c r="AH43" s="18">
-        <f t="shared" si="33"/>
-        <v>0.24072753209700432</v>
-      </c>
-      <c r="AI43" s="18">
-        <f t="shared" si="34"/>
-        <v>0.75927246790299563</v>
-      </c>
-      <c r="AJ43" s="18">
-        <v>0.34799999999999998</v>
-      </c>
-      <c r="AK43" s="18">
-        <v>2.984</v>
-      </c>
-      <c r="AL43" s="18">
-        <f t="shared" si="35"/>
-        <v>0.11662198391420911</v>
-      </c>
-      <c r="AM43" s="18">
-        <f t="shared" si="36"/>
-        <v>0.88337801608579092</v>
-      </c>
-      <c r="AN43" s="18">
-        <v>0.502</v>
-      </c>
-      <c r="AO43" s="18">
-        <f t="shared" si="20"/>
-        <v>3.1360000000000001</v>
-      </c>
-      <c r="AP43" s="18">
-        <f t="shared" si="37"/>
-        <v>0.16007653061224489</v>
-      </c>
-      <c r="AQ43" s="18">
-        <f t="shared" si="38"/>
-        <v>0.83992346938775508</v>
-      </c>
-      <c r="AR43" s="18">
-        <f t="shared" si="39"/>
-        <v>0.65427229891890515</v>
-      </c>
-    </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F44" s="18">
-        <v>0.35899999999999999</v>
-      </c>
-      <c r="G44" s="18">
-        <v>3.6070000000000002</v>
-      </c>
-      <c r="H44" s="18">
-        <f t="shared" si="21"/>
-        <v>9.9528694205711102E-2</v>
-      </c>
-      <c r="I44" s="18">
-        <f t="shared" si="22"/>
-        <v>0.90047130579428891</v>
-      </c>
-      <c r="J44" s="18">
-        <v>1.25</v>
-      </c>
-      <c r="K44" s="18">
-        <v>1.03</v>
-      </c>
-      <c r="L44" s="18">
-        <v>2.032</v>
-      </c>
-      <c r="M44" s="18">
-        <v>3.786</v>
-      </c>
-      <c r="N44" s="18">
-        <f t="shared" si="23"/>
-        <v>5.8179999999999996</v>
-      </c>
-      <c r="O44" s="18">
-        <f t="shared" si="24"/>
-        <v>0.21485046407700242</v>
-      </c>
-      <c r="P44" s="18">
-        <f t="shared" si="25"/>
-        <v>0.78514953592299763</v>
-      </c>
-      <c r="Q44" s="18">
-        <v>1.546</v>
-      </c>
-      <c r="R44" s="18">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="S44" s="18">
-        <v>2.544</v>
-      </c>
-      <c r="T44" s="18">
-        <v>0.64200000000000002</v>
-      </c>
-      <c r="U44" s="18">
-        <f t="shared" si="26"/>
-        <v>3.1859999999999999</v>
-      </c>
-      <c r="V44" s="18">
-        <f t="shared" si="27"/>
-        <v>0.48524795982423102</v>
-      </c>
-      <c r="W44" s="18">
-        <f t="shared" si="28"/>
-        <v>0.51475204017576903</v>
-      </c>
-      <c r="X44" s="18">
-        <v>0.24</v>
-      </c>
-      <c r="Y44" s="18">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="Z44" s="18">
-        <f t="shared" si="29"/>
-        <v>9.1529999999999987</v>
-      </c>
-      <c r="AA44" s="18">
-        <f t="shared" si="30"/>
-        <v>1.6278815688845188E-2</v>
-      </c>
-      <c r="AB44" s="18">
-        <v>0.44800000000000001</v>
-      </c>
-      <c r="AC44" s="18">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="AD44" s="18">
-        <f t="shared" si="31"/>
-        <v>0.46473029045643155</v>
-      </c>
-      <c r="AE44" s="18">
-        <f t="shared" si="32"/>
-        <v>0.53526970954356845</v>
-      </c>
-      <c r="AF44" s="18">
-        <v>0.41399999999999998</v>
-      </c>
-      <c r="AG44" s="18">
-        <f t="shared" si="19"/>
-        <v>1.25</v>
-      </c>
-      <c r="AH44" s="18">
-        <f t="shared" si="33"/>
-        <v>0.33119999999999999</v>
-      </c>
-      <c r="AI44" s="18">
-        <f t="shared" si="34"/>
-        <v>0.66880000000000006</v>
-      </c>
-      <c r="AJ44" s="18">
-        <v>0.246</v>
-      </c>
-      <c r="AK44" s="18">
-        <v>1.472</v>
-      </c>
-      <c r="AL44" s="18">
-        <f t="shared" si="35"/>
-        <v>0.1671195652173913</v>
-      </c>
-      <c r="AM44" s="18">
-        <f t="shared" si="36"/>
-        <v>0.83288043478260865</v>
-      </c>
-      <c r="AN44" s="18">
-        <v>0.27100000000000002</v>
-      </c>
-      <c r="AO44" s="18">
-        <f t="shared" si="20"/>
-        <v>1.546</v>
-      </c>
-      <c r="AP44" s="18">
-        <f t="shared" si="37"/>
-        <v>0.17529107373868047</v>
-      </c>
-      <c r="AQ44" s="18">
-        <f t="shared" si="38"/>
-        <v>0.82470892626131953</v>
-      </c>
-      <c r="AR44" s="18">
-        <f t="shared" si="39"/>
-        <v>0.63478884602117469</v>
-      </c>
-    </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F45" s="18">
-        <v>0.156</v>
-      </c>
-      <c r="G45" s="18">
-        <v>1.3240000000000001</v>
-      </c>
-      <c r="H45" s="18">
-        <f t="shared" si="21"/>
-        <v>0.11782477341389727</v>
-      </c>
-      <c r="I45" s="18">
-        <f t="shared" si="22"/>
-        <v>0.8821752265861027</v>
-      </c>
-      <c r="J45" s="18">
-        <v>1.7689999999999999</v>
-      </c>
-      <c r="K45" s="18">
-        <v>0.77300000000000002</v>
-      </c>
-      <c r="L45" s="18">
-        <v>1.9430000000000001</v>
-      </c>
-      <c r="M45" s="18">
-        <v>1.645</v>
-      </c>
-      <c r="N45" s="18">
-        <f t="shared" si="23"/>
-        <v>3.5880000000000001</v>
-      </c>
-      <c r="O45" s="18">
-        <f t="shared" si="24"/>
-        <v>0.49303232998885171</v>
-      </c>
-      <c r="P45" s="18">
-        <f t="shared" si="25"/>
-        <v>0.50696767001114829</v>
-      </c>
-      <c r="Q45" s="18">
-        <v>1.228</v>
-      </c>
-      <c r="R45" s="18">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="S45" s="18">
-        <v>1.7649999999999999</v>
-      </c>
-      <c r="T45" s="18">
-        <v>0.373</v>
-      </c>
-      <c r="U45" s="18">
-        <f t="shared" si="26"/>
-        <v>2.1379999999999999</v>
-      </c>
-      <c r="V45" s="18">
-        <f t="shared" si="27"/>
-        <v>0.57436856875584663</v>
-      </c>
-      <c r="W45" s="18">
-        <f t="shared" si="28"/>
-        <v>0.42563143124415337</v>
-      </c>
-      <c r="X45" s="18">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="Y45" s="18">
-        <v>0.78900000000000003</v>
-      </c>
-      <c r="Z45" s="18">
-        <f t="shared" si="29"/>
-        <v>6.5149999999999997</v>
-      </c>
-      <c r="AA45" s="18">
-        <f t="shared" si="30"/>
-        <v>0.12110514198004606</v>
-      </c>
-      <c r="AB45" s="18">
-        <v>0.34200000000000003</v>
-      </c>
-      <c r="AC45" s="18">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="AD45" s="18">
-        <f t="shared" si="31"/>
-        <v>0.382122905027933</v>
-      </c>
-      <c r="AE45" s="18">
-        <f t="shared" si="32"/>
-        <v>0.617877094972067</v>
-      </c>
-      <c r="AF45" s="18">
-        <v>0.31900000000000001</v>
-      </c>
-      <c r="AG45" s="18">
-        <f t="shared" si="19"/>
-        <v>1.7689999999999999</v>
-      </c>
-      <c r="AH45" s="18">
-        <f t="shared" si="33"/>
-        <v>0.18032786885245902</v>
-      </c>
-      <c r="AI45" s="18">
-        <f t="shared" si="34"/>
-        <v>0.81967213114754101</v>
-      </c>
-      <c r="AJ45" s="18">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="AK45" s="18">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="AL45" s="18">
-        <f t="shared" si="35"/>
-        <v>0.19938650306748468</v>
-      </c>
-      <c r="AM45" s="18">
-        <f t="shared" si="36"/>
-        <v>0.80061349693251538</v>
-      </c>
-      <c r="AN45" s="18">
-        <v>0.372</v>
-      </c>
-      <c r="AO45" s="18">
-        <f t="shared" si="20"/>
-        <v>1.228</v>
-      </c>
-      <c r="AP45" s="18">
-        <f t="shared" si="37"/>
-        <v>0.30293159609120524</v>
-      </c>
-      <c r="AQ45" s="18">
-        <f t="shared" si="38"/>
-        <v>0.69706840390879476</v>
-      </c>
-      <c r="AR45" s="18">
-        <f t="shared" si="39"/>
-        <v>0.60888882459779603</v>
-      </c>
-      <c r="AT45" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F46" s="18">
-        <v>0.24</v>
-      </c>
-      <c r="G46" s="18">
-        <v>1.57</v>
-      </c>
-      <c r="H46" s="18">
-        <f t="shared" si="21"/>
-        <v>0.15286624203821655</v>
-      </c>
-      <c r="I46" s="18">
-        <f t="shared" si="22"/>
-        <v>0.84713375796178347</v>
-      </c>
-      <c r="J46" s="18">
-        <v>1.3660000000000001</v>
-      </c>
-      <c r="K46" s="18">
-        <v>0.99199999999999999</v>
-      </c>
-      <c r="L46" s="18">
-        <v>1.5669999999999999</v>
-      </c>
-      <c r="M46" s="18">
-        <v>2.214</v>
-      </c>
-      <c r="N46" s="18">
-        <f t="shared" si="23"/>
-        <v>3.7809999999999997</v>
-      </c>
-      <c r="O46" s="18">
-        <f t="shared" si="24"/>
-        <v>0.36128008463369482</v>
-      </c>
-      <c r="P46" s="18">
-        <f t="shared" si="25"/>
-        <v>0.63871991536630524</v>
-      </c>
-      <c r="Q46" s="18">
-        <v>1.1220000000000001</v>
-      </c>
-      <c r="R46" s="18">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="S46" s="18">
-        <v>4.2350000000000003</v>
-      </c>
-      <c r="T46" s="18">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="U46" s="18">
-        <f t="shared" si="26"/>
-        <v>4.91</v>
-      </c>
-      <c r="V46" s="18">
-        <f t="shared" si="27"/>
-        <v>0.22851323828920572</v>
-      </c>
-      <c r="W46" s="18">
-        <f t="shared" si="28"/>
-        <v>0.77148676171079433</v>
-      </c>
-      <c r="X46" s="18">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="Y46" s="18">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="Z46" s="18">
-        <f t="shared" si="29"/>
-        <v>8.7890000000000015</v>
-      </c>
-      <c r="AA46" s="18">
-        <f t="shared" si="30"/>
-        <v>1.1150301513255204E-2</v>
-      </c>
-      <c r="AB46" s="18">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="AC46" s="18">
-        <v>0.93899999999999995</v>
-      </c>
-      <c r="AD46" s="18">
-        <f t="shared" si="31"/>
-        <v>0.37912673056443025</v>
-      </c>
-      <c r="AE46" s="18">
-        <f t="shared" si="32"/>
-        <v>0.62087326943556975</v>
-      </c>
-      <c r="AF46" s="18">
-        <v>0.46899999999999997</v>
-      </c>
-      <c r="AG46" s="18">
-        <f t="shared" si="19"/>
-        <v>1.3660000000000001</v>
-      </c>
-      <c r="AH46" s="18">
-        <f t="shared" si="33"/>
-        <v>0.3433382137628111</v>
-      </c>
-      <c r="AI46" s="18">
-        <f t="shared" si="34"/>
-        <v>0.65666178623718885</v>
-      </c>
-      <c r="AJ46" s="18">
-        <v>0.33900000000000002</v>
-      </c>
-      <c r="AK46" s="18">
-        <v>1.0740000000000001</v>
-      </c>
-      <c r="AL46" s="18">
-        <f t="shared" si="35"/>
-        <v>0.31564245810055869</v>
-      </c>
-      <c r="AM46" s="18">
-        <f t="shared" si="36"/>
-        <v>0.68435754189944131</v>
-      </c>
-      <c r="AN46" s="18">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="AO46" s="18">
-        <f t="shared" si="20"/>
-        <v>1.1220000000000001</v>
-      </c>
-      <c r="AP46" s="18">
-        <f t="shared" si="37"/>
-        <v>0.24598930481283421</v>
-      </c>
-      <c r="AQ46" s="18">
-        <f t="shared" si="38"/>
-        <v>0.75401069518716579</v>
-      </c>
-      <c r="AR46" s="18">
-        <f t="shared" si="39"/>
-        <v>0.62304925366393804</v>
-      </c>
-    </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F47" s="18">
-        <v>0.224</v>
-      </c>
-      <c r="G47" s="18">
-        <v>1.2050000000000001</v>
-      </c>
-      <c r="H47" s="18">
-        <f t="shared" si="21"/>
-        <v>0.18589211618257262</v>
-      </c>
-      <c r="I47" s="18">
-        <f t="shared" si="22"/>
-        <v>0.81410788381742738</v>
-      </c>
-      <c r="J47" s="18">
-        <v>1.71</v>
-      </c>
-      <c r="K47" s="18">
-        <v>1.022</v>
-      </c>
-      <c r="L47" s="18">
-        <v>1.8420000000000001</v>
-      </c>
-      <c r="M47" s="18">
-        <v>2.4380000000000002</v>
-      </c>
-      <c r="N47" s="18">
-        <f t="shared" si="23"/>
-        <v>4.28</v>
-      </c>
-      <c r="O47" s="18">
-        <f t="shared" si="24"/>
-        <v>0.39953271028037379</v>
-      </c>
-      <c r="P47" s="18">
-        <f t="shared" si="25"/>
-        <v>0.60046728971962615</v>
-      </c>
-      <c r="Q47" s="18">
-        <v>1.327</v>
-      </c>
-      <c r="R47" s="18">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="S47" s="18">
-        <v>3.1840000000000002</v>
-      </c>
-      <c r="T47" s="18">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="U47" s="18">
-        <f t="shared" si="26"/>
-        <v>4.0150000000000006</v>
-      </c>
-      <c r="V47" s="18">
-        <f t="shared" si="27"/>
-        <v>0.3305105853051058</v>
-      </c>
-      <c r="W47" s="18">
-        <f t="shared" si="28"/>
-        <v>0.6694894146948942</v>
-      </c>
-      <c r="X47" s="18">
-        <v>0.20599999999999999</v>
-      </c>
-      <c r="Y47" s="18">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="Z47" s="18">
-        <f t="shared" si="29"/>
-        <v>8.4580000000000002</v>
-      </c>
-      <c r="AA47" s="18">
-        <f t="shared" si="30"/>
-        <v>1.9271695436273353E-2</v>
-      </c>
-      <c r="AB47" s="18">
-        <v>0.41299999999999998</v>
-      </c>
-      <c r="AC47" s="18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AD47" s="18">
-        <f t="shared" si="31"/>
-        <v>0.37545454545454543</v>
-      </c>
-      <c r="AE47" s="18">
-        <f t="shared" si="32"/>
-        <v>0.62454545454545451</v>
-      </c>
-      <c r="AF47" s="18">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="AG47" s="18">
-        <f t="shared" si="19"/>
-        <v>1.71</v>
-      </c>
-      <c r="AH47" s="18">
-        <f t="shared" si="33"/>
-        <v>0.31988304093567255</v>
-      </c>
-      <c r="AI47" s="18">
-        <f t="shared" si="34"/>
-        <v>0.68011695906432745</v>
-      </c>
-      <c r="AJ47" s="18">
-        <v>0.505</v>
-      </c>
-      <c r="AK47" s="18">
-        <v>1.1160000000000001</v>
-      </c>
-      <c r="AL47" s="18">
-        <f t="shared" si="35"/>
-        <v>0.45250896057347667</v>
-      </c>
-      <c r="AM47" s="18">
-        <f t="shared" si="36"/>
-        <v>0.54749103942652333</v>
-      </c>
-      <c r="AN47" s="18">
-        <v>0.628</v>
-      </c>
-      <c r="AO47" s="18">
-        <f t="shared" si="20"/>
-        <v>1.327</v>
-      </c>
-      <c r="AP47" s="18">
-        <f t="shared" si="37"/>
-        <v>0.47324792765636775</v>
-      </c>
-      <c r="AQ47" s="18">
-        <f t="shared" si="38"/>
-        <v>0.5267520723436323</v>
-      </c>
-      <c r="AR47" s="18">
-        <f t="shared" si="39"/>
-        <v>0.5602802261310198</v>
-      </c>
-    </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F48" s="18">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="G48" s="18">
-        <v>0.628</v>
-      </c>
-      <c r="H48" s="18">
-        <f t="shared" si="21"/>
-        <v>0.13853503184713375</v>
-      </c>
-      <c r="I48" s="18">
-        <f t="shared" si="22"/>
-        <v>0.86146496815286622</v>
-      </c>
-      <c r="J48" s="18">
-        <v>0.76400000000000001</v>
-      </c>
-      <c r="K48" s="18">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="L48" s="18">
-        <v>0.80900000000000005</v>
-      </c>
-      <c r="M48" s="18">
-        <v>1.0249999999999999</v>
-      </c>
-      <c r="N48" s="18">
-        <f t="shared" si="23"/>
-        <v>1.8340000000000001</v>
-      </c>
-      <c r="O48" s="18">
-        <f t="shared" si="24"/>
-        <v>0.41657579062159211</v>
-      </c>
-      <c r="P48" s="18">
-        <f t="shared" si="25"/>
-        <v>0.58342420937840789</v>
-      </c>
-      <c r="Q48" s="18">
-        <v>0.81100000000000005</v>
-      </c>
-      <c r="R48" s="18">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="S48" s="18">
-        <v>0.999</v>
-      </c>
-      <c r="T48" s="18">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="U48" s="18">
-        <f t="shared" si="26"/>
-        <v>1.1759999999999999</v>
-      </c>
-      <c r="V48" s="18">
-        <f t="shared" si="27"/>
-        <v>0.68962585034013613</v>
-      </c>
-      <c r="W48" s="18">
-        <f t="shared" si="28"/>
-        <v>0.31037414965986387</v>
-      </c>
-      <c r="X48" s="18">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="Y48" s="18">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="Z48" s="18">
-        <f t="shared" si="29"/>
-        <v>3.0640000000000001</v>
-      </c>
-      <c r="AA48" s="18">
-        <f t="shared" si="30"/>
-        <v>1.7624020887728457E-2</v>
-      </c>
-      <c r="AB48" s="18">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="AC48" s="18">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="AD48" s="18">
-        <f t="shared" si="31"/>
-        <v>0.28515625</v>
-      </c>
-      <c r="AE48" s="18">
-        <f t="shared" si="32"/>
-        <v>0.71484375</v>
-      </c>
-      <c r="AF48" s="18">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="AG48" s="18">
-        <f t="shared" si="19"/>
-        <v>0.76400000000000001</v>
-      </c>
-      <c r="AH48" s="18">
-        <f t="shared" si="33"/>
-        <v>0.21989528795811519</v>
-      </c>
-      <c r="AI48" s="18">
-        <f t="shared" si="34"/>
-        <v>0.78010471204188481</v>
-      </c>
-      <c r="AJ48" s="18">
-        <v>0.153</v>
-      </c>
-      <c r="AK48" s="18">
-        <v>0.64400000000000002</v>
-      </c>
-      <c r="AL48" s="18">
-        <f t="shared" si="35"/>
-        <v>0.23757763975155277</v>
-      </c>
-      <c r="AM48" s="18">
-        <f t="shared" si="36"/>
-        <v>0.76242236024844723</v>
-      </c>
-      <c r="AN48" s="18">
-        <v>0.11</v>
-      </c>
-      <c r="AO48" s="18">
-        <f t="shared" si="20"/>
-        <v>0.81100000000000005</v>
-      </c>
-      <c r="AP48" s="18">
-        <f t="shared" si="37"/>
-        <v>0.13563501849568432</v>
-      </c>
-      <c r="AQ48" s="18">
-        <f t="shared" si="38"/>
-        <v>0.86436498150431573</v>
-      </c>
-      <c r="AR48" s="18">
-        <f t="shared" si="39"/>
-        <v>0.61182789398418924</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C22" r:id="rId1" tooltip="Formicinae" display="https://en.wikipedia.org/wiki/Formicinae" xr:uid="{F29564A9-5B32-43A7-86E4-E3EF73DCC7BD}"/>
-    <hyperlink ref="C20" r:id="rId2" tooltip="Formicinae" display="https://en.wikipedia.org/wiki/Formicinae" xr:uid="{EAE96AC8-58BF-4D25-9050-5C3347AEB828}"/>
-    <hyperlink ref="C21" r:id="rId3" tooltip="Formicinae" display="https://en.wikipedia.org/wiki/Formicinae" xr:uid="{7ED61731-9773-4B7E-BC24-1D59429DE082}"/>
+    <hyperlink ref="C22" r:id="rId1" tooltip="Formicinae" display="https://en.wikipedia.org/wiki/Formicinae"/>
+    <hyperlink ref="C20" r:id="rId2" tooltip="Formicinae" display="https://en.wikipedia.org/wiki/Formicinae"/>
+    <hyperlink ref="C21" r:id="rId3" tooltip="Formicinae" display="https://en.wikipedia.org/wiki/Formicinae"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>